<commit_message>
updated BOM with more details
</commit_message>
<xml_diff>
--- a/Hardware/McuOpenPnP Bill of Material.xlsx
+++ b/Hardware/McuOpenPnP Bill of Material.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66A07BAC-F185-41A6-95BA-89156E4ADBA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>McuOpenPnP Machine Bill of Material</t>
   </si>
@@ -49,9 +50,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>You need lots of them, in different sizes</t>
-  </si>
-  <si>
     <t>M5 T-Nuts</t>
   </si>
   <si>
@@ -190,9 +188,6 @@
     <t>Smoothieboard LCD Adapter</t>
   </si>
   <si>
-    <t>USB Cameras</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/720P-CMOS-micro-mini-usb-camera-board-for-android-windows-linux-equipment-manufacturers-ELP-USB100W03M-L60/32346777227.html</t>
   </si>
   <si>
@@ -241,9 +236,6 @@
     <t>Samsung CP40 Holder 5 mm Screw</t>
   </si>
   <si>
-    <t>LED Ring 60 mm 24V</t>
-  </si>
-  <si>
     <t>Distrelec</t>
   </si>
   <si>
@@ -362,12 +354,33 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/Full-Graphic-Smart-Controller-LCD-Display-for-RAMPS-1-4-RepRap-3D-Printer-Electronics-12864-display/32852039927.html?spm=2114.search0104.3.50.36d453aeuCGxi0&amp;ws_ab_test=searchweb0_0,searchweb201602_5_10846_10152_10065_10151_10344_10068_10342_10343_10340_10059_10341_10696_100031_10084_10083_10103_524_10618_10307_10624_10623_10622_10621_10620_10134,searchweb201603_35,ppcSwitch_4&amp;algo_expid=a277e213-a8b6-4e11-92a8-a214f019869e-7&amp;algo_pvid=a277e213-a8b6-4e11-92a8-a214f019869e&amp;transAbTest=ae803_2&amp;priceBeautifyAB=0</t>
+  </si>
+  <si>
+    <t>LED Ring 60 mm 24V, white</t>
+  </si>
+  <si>
+    <t>Optional, order 45cm if 42.5 is not available</t>
+  </si>
+  <si>
+    <t>Optional, used in the build to attach the frame to the ground plate</t>
+  </si>
+  <si>
+    <t>Better order a few more</t>
+  </si>
+  <si>
+    <t>You need lots of them, with different length</t>
+  </si>
+  <si>
+    <t>USB Camera OV9712, 6 mm Lens</t>
+  </si>
+  <si>
+    <t>You want a 6mm lens, 3.6 or 2.1 is too fisheye</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,7 +476,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -479,9 +492,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -519,9 +532,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,9 +567,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,9 +619,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,14 +811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
@@ -789,7 +836,7 @@
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="D2" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="12">
         <f>SUM(E4:E66)</f>
@@ -821,10 +868,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -837,16 +884,19 @@
         <f>C4*D4</f>
         <v>9.5399999999999991</v>
       </c>
+      <c r="F4" t="s">
+        <v>116</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -859,16 +909,19 @@
         <f>C5*D5</f>
         <v>9.5299999999999994</v>
       </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>40</v>
@@ -881,16 +934,19 @@
         <f>C6*D6</f>
         <v>23.96</v>
       </c>
+      <c r="F6" t="s">
+        <v>116</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -904,15 +960,15 @@
         <v>66.680000000000007</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -925,15 +981,15 @@
         <v>19.2</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -946,15 +1002,15 @@
         <v>3.45</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -967,15 +1023,15 @@
         <v>37.9</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -988,15 +1044,15 @@
         <v>28</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1009,15 +1065,15 @@
         <v>66.56</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1030,15 +1086,15 @@
         <v>10.8</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -1051,18 +1107,18 @@
         <v>16.799999999999997</v>
       </c>
       <c r="F14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1075,18 +1131,18 @@
         <v>3.25</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1099,18 +1155,18 @@
         <v>5.32</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -1124,18 +1180,18 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1148,18 +1204,18 @@
         <v>9.5</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1172,18 +1228,18 @@
         <v>33.700000000000003</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1196,18 +1252,18 @@
         <v>5.5</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -1220,18 +1276,18 @@
         <v>35</v>
       </c>
       <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1244,15 +1300,15 @@
         <v>50</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -1266,18 +1322,18 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1291,18 +1347,18 @@
         <v>1.56</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1315,18 +1371,18 @@
         <v>34.58</v>
       </c>
       <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1339,15 +1395,15 @@
         <v>204</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1360,18 +1416,18 @@
         <v>25.45</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1384,16 +1440,19 @@
         <f t="shared" si="0"/>
         <v>57.78</v>
       </c>
+      <c r="F28" t="s">
+        <v>119</v>
+      </c>
       <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1407,15 +1466,15 @@
         <v>10.3</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1429,15 +1488,15 @@
         <v>29.19</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1450,16 +1509,19 @@
         <f t="shared" si="0"/>
         <v>18.399999999999999</v>
       </c>
+      <c r="F31" t="s">
+        <v>114</v>
+      </c>
       <c r="G31" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1473,18 +1535,18 @@
         <v>14.17</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1498,18 +1560,18 @@
         <v>1.94</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1523,15 +1585,15 @@
         <v>6.62</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1544,18 +1606,18 @@
         <v>43.6</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1568,18 +1630,18 @@
         <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1592,18 +1654,18 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1616,15 +1678,15 @@
         <v>0.6</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1637,15 +1699,15 @@
         <v>1.6</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1658,15 +1720,15 @@
         <v>7.2</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1679,7 +1741,7 @@
         <v>7.1999999999999993</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,7 +1752,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1698,12 +1760,12 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -1711,7 +1773,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1724,7 +1786,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1737,12 +1799,12 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -1750,12 +1812,12 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -1763,23 +1825,23 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -1791,12 +1853,12 @@
         <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -1808,46 +1870,46 @@
         <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="G7" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6"/>
-    <hyperlink ref="G11" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G13" r:id="rId9"/>
-    <hyperlink ref="G20" r:id="rId10"/>
-    <hyperlink ref="G19" r:id="rId11"/>
-    <hyperlink ref="G22" r:id="rId12"/>
-    <hyperlink ref="G21" r:id="rId13"/>
-    <hyperlink ref="G23" r:id="rId14"/>
-    <hyperlink ref="G26" r:id="rId15"/>
-    <hyperlink ref="G28" r:id="rId16"/>
-    <hyperlink ref="G31" r:id="rId17"/>
-    <hyperlink ref="G30" r:id="rId18"/>
-    <hyperlink ref="G32" r:id="rId19"/>
-    <hyperlink ref="G29" r:id="rId20"/>
-    <hyperlink ref="G33" r:id="rId21"/>
-    <hyperlink ref="G34" r:id="rId22"/>
-    <hyperlink ref="G25" r:id="rId23"/>
-    <hyperlink ref="G27" r:id="rId24"/>
-    <hyperlink ref="G35" r:id="rId25"/>
-    <hyperlink ref="G39" r:id="rId26"/>
-    <hyperlink ref="G37" r:id="rId27"/>
-    <hyperlink ref="G36" r:id="rId28"/>
-    <hyperlink ref="G38" r:id="rId29"/>
-    <hyperlink ref="G40" r:id="rId30"/>
-    <hyperlink ref="G41" r:id="rId31"/>
-    <hyperlink ref="G24" r:id="rId32"/>
-    <hyperlink ref="G14" r:id="rId33"/>
-    <hyperlink ref="G15" r:id="rId34"/>
-    <hyperlink ref="G16" r:id="rId35"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G22" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G26" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G36" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G40" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G41" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G24" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G14" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G15" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G16" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId36"/>

</xml_diff>

<commit_message>
updated number of idlers
</commit_message>
<xml_diff>
--- a/Hardware/McuOpenPnP Bill of Material.xlsx
+++ b/Hardware/McuOpenPnP Bill of Material.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66A07BAC-F185-41A6-95BA-89156E4ADBA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="121">
   <si>
     <t>McuOpenPnP Machine Bill of Material</t>
   </si>
@@ -375,12 +374,15 @@
   </si>
   <si>
     <t>You want a 6mm lens, 3.6 or 2.1 is too fisheye</t>
+  </si>
+  <si>
+    <t>Depends on your configuration. You need at least 3.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,7 +478,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -492,9 +494,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -532,9 +534,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,26 +569,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -619,26 +604,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -811,14 +779,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
@@ -840,7 +808,7 @@
       </c>
       <c r="E2" s="12">
         <f>SUM(E4:E66)</f>
-        <v>970.88000000000011</v>
+        <v>974.48</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1710,14 +1678,17 @@
         <v>26</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D40" s="6">
         <v>1.8</v>
       </c>
       <c r="E40" s="6">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>10.8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>120</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>79</v>
@@ -1875,41 +1846,41 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G22" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G26" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G36" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G40" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G41" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G24" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G14" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G15" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G16" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G5" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G8" r:id="rId5"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G11" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="G13" r:id="rId9"/>
+    <hyperlink ref="G20" r:id="rId10"/>
+    <hyperlink ref="G19" r:id="rId11"/>
+    <hyperlink ref="G22" r:id="rId12"/>
+    <hyperlink ref="G21" r:id="rId13"/>
+    <hyperlink ref="G23" r:id="rId14"/>
+    <hyperlink ref="G26" r:id="rId15"/>
+    <hyperlink ref="G28" r:id="rId16"/>
+    <hyperlink ref="G31" r:id="rId17"/>
+    <hyperlink ref="G30" r:id="rId18"/>
+    <hyperlink ref="G32" r:id="rId19"/>
+    <hyperlink ref="G29" r:id="rId20"/>
+    <hyperlink ref="G33" r:id="rId21"/>
+    <hyperlink ref="G34" r:id="rId22"/>
+    <hyperlink ref="G25" r:id="rId23"/>
+    <hyperlink ref="G27" r:id="rId24"/>
+    <hyperlink ref="G35" r:id="rId25"/>
+    <hyperlink ref="G39" r:id="rId26"/>
+    <hyperlink ref="G37" r:id="rId27"/>
+    <hyperlink ref="G36" r:id="rId28"/>
+    <hyperlink ref="G38" r:id="rId29"/>
+    <hyperlink ref="G40" r:id="rId30"/>
+    <hyperlink ref="G41" r:id="rId31"/>
+    <hyperlink ref="G24" r:id="rId32"/>
+    <hyperlink ref="G14" r:id="rId33"/>
+    <hyperlink ref="G15" r:id="rId34"/>
+    <hyperlink ref="G16" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId36"/>

</xml_diff>